<commit_message>
Update to code for better performances
</commit_message>
<xml_diff>
--- a/TirageTombola/FichiersExcel/Liste des lots.xlsx
+++ b/TirageTombola/FichiersExcel/Liste des lots.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr date1904="1" filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C693ED-0FA7-40E0-82A5-C4928FDE3AF0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E94F586-1B76-43E1-B93D-CD518D6066C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19545" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10230" yWindow="3930" windowWidth="27840" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lots" sheetId="1" r:id="rId1"/>
     <sheet name="Programmes gagnants" sheetId="2" r:id="rId2"/>
-    <sheet name="Hypthèses programmes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
   <si>
     <t>Lot de boules de Noël</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -157,12 +157,6 @@
   </si>
   <si>
     <t>Entrez le numero du programme:</t>
-  </si>
-  <si>
-    <t>Numero programme max</t>
-  </si>
-  <si>
-    <t>Numeros des programmes non vendus</t>
   </si>
   <si>
     <t>Cadre photo horloge</t>
@@ -735,7 +729,9 @@
   <sheetPr published="0"/>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -754,7 +750,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -763,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -772,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -799,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -808,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -817,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -826,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -835,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -844,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -853,7 +849,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -916,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -925,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -991,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1003,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -1015,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -1027,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -1039,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -1051,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -1063,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D33" s="1"/>
     </row>
@@ -1075,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -1087,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" s="1"/>
     </row>
@@ -1117,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -1129,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D39" s="1"/>
     </row>
@@ -1141,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D40" s="1"/>
     </row>
@@ -1153,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -1375,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D60" s="1"/>
     </row>
@@ -1584,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D78" s="1"/>
     </row>
@@ -1596,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D79" s="1"/>
     </row>
@@ -1608,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D80" s="1"/>
     </row>
@@ -1620,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D81" s="1"/>
     </row>
@@ -1632,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D82" s="1"/>
     </row>
@@ -1644,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D83" s="1"/>
     </row>
@@ -1656,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D84" s="1"/>
     </row>
@@ -1668,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D85" s="1"/>
     </row>
@@ -1680,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D86" s="1"/>
     </row>
@@ -1692,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D87" s="1"/>
     </row>
@@ -1704,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D88" s="1"/>
     </row>
@@ -1716,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D89" s="1"/>
     </row>
@@ -1728,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D90" s="1"/>
     </row>
@@ -1740,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D91" s="1"/>
     </row>
@@ -1750,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D92" s="1"/>
     </row>
@@ -1767,7 +1763,7 @@
       <c r="C101" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="C62:C91">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C62:C91">
     <sortCondition ref="C62:C91"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1836,66 +1832,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr published="0"/>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.25" customWidth="1"/>
-    <col min="2" max="2" width="36.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>300</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>